<commit_message>
edited the mapping spreadsheet
</commit_message>
<xml_diff>
--- a/data/mapping.xlsx
+++ b/data/mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Jobs\Freelancing\Upwork\061 - Interscript - Ribose - Ronald Tse\Code stuff\005 - Mapping the PoS tagging system used in Hazm to the one in 50k+ dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Jobs\Freelancing\Upwork\061 - Interscript - Ribose - Ronald Tse\Code stuff\003 - Rababa\rababa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB541EE-0550-45FD-996B-3088D552E90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAF82F0-6265-4CB0-83A7-F5CF4ABE997C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,16 +108,16 @@
     <t>Sp, NA</t>
   </si>
   <si>
-    <t>N5, N6, N7, N8, (NA)</t>
-  </si>
-  <si>
-    <t>Po, (N9), Pr, Pr1</t>
-  </si>
-  <si>
-    <t>V1, V2, V3, V4, V5, (VPr)</t>
-  </si>
-  <si>
-    <t>N1, N2, N3, N4, N9, ((NA)), VPr</t>
+    <t>N1, N2, N3, N4, N9, NA, VPr</t>
+  </si>
+  <si>
+    <t>V1, V2, V3, V4, V5, VPr</t>
+  </si>
+  <si>
+    <t>Po, N9, Pr, Pr1</t>
+  </si>
+  <si>
+    <t>N5, N6, N7, N8, NA</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -488,7 +488,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -573,7 +573,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>

</xml_diff>